<commit_message>
Changed testing website and fixed formatting to be PEP8 compliant
</commit_message>
<xml_diff>
--- a/TestData/logindata.xlsx
+++ b/TestData/logindata.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Limi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Limi\PycharmProjects\pythonBaseFramework\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{204B8080-E210-4D4B-B9FF-72C148C25C86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6892D48D-0890-427D-B560-07B125BC02A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
   <si>
     <t>username</t>
   </si>
@@ -36,31 +36,31 @@
     <t>exp</t>
   </si>
   <si>
-    <t>bojar47999@iucake.com</t>
-  </si>
-  <si>
-    <t>dudettewoman12</t>
-  </si>
-  <si>
     <t>pass</t>
   </si>
   <si>
-    <t>dude</t>
-  </si>
-  <si>
-    <t>man</t>
-  </si>
-  <si>
     <t>fail</t>
   </si>
   <si>
-    <t>e</t>
-  </si>
-  <si>
     <t>fdafasdfa</t>
   </si>
   <si>
     <t>dasdaew</t>
+  </si>
+  <si>
+    <t>standard_user</t>
+  </si>
+  <si>
+    <t>secret_sauce</t>
+  </si>
+  <si>
+    <t>locked_out_user</t>
+  </si>
+  <si>
+    <t>problem_user</t>
+  </si>
+  <si>
+    <t>performance_glitch_user</t>
   </si>
 </sst>
 </file>
@@ -117,10 +117,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -401,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -426,46 +427,57 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="B6" s="3" t="s">
         <v>8</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added screenshot on failure
</commit_message>
<xml_diff>
--- a/TestData/logindata.xlsx
+++ b/TestData/logindata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Limi\PycharmProjects\pythonBaseFramework\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6892D48D-0890-427D-B560-07B125BC02A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77DEE4D6-A2D1-4090-AEEC-DB84C39F5869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -405,7 +405,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Modified DDT test login and added cart page object
</commit_message>
<xml_diff>
--- a/TestData/logindata.xlsx
+++ b/TestData/logindata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Limi\PycharmProjects\pythonBaseFramework\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA5AC3FA-8A23-4465-B3B5-CF43C2E5CA90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94178A68-EB7C-4CB4-B631-EA8549DDA6DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6615" yWindow="2355" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="13">
   <si>
     <t>username</t>
   </si>
@@ -405,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -452,45 +452,81 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
+      <c r="A5" s="1"/>
+      <c r="B5" s="1">
+        <v>1234</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="C10" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>